<commit_message>
Fixed current date vs first screen date issue, added loggers, and fixed birthday processing
</commit_message>
<xml_diff>
--- a/database/WVHA Outcomes (Database).xlsx
+++ b/database/WVHA Outcomes (Database).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorakolo/Desktop/HHI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorakolo/Desktop/HHI/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA347D-4B1C-F84D-AD3E-4D10CADFBC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E92E98E-B1DF-114D-A52A-9565D8D2B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37360" yWindow="500" windowWidth="34300" windowHeight="18540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35740" yWindow="1140" windowWidth="34300" windowHeight="18540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENT LIST" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="342">
   <si>
     <t>HRA</t>
   </si>
@@ -1173,6 +1173,9 @@
   </si>
   <si>
     <t>A1C.1</t>
+  </si>
+  <si>
+    <t>FASTING.1</t>
   </si>
 </sst>
 </file>
@@ -3441,257 +3444,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3731,6 +3483,278 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3745,27 +3769,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="39" fontId="31" fillId="27" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8618,10 +8621,10 @@
   </sheetPr>
   <dimension ref="A1:BW802"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8825,7 +8828,7 @@
         <v>27</v>
       </c>
       <c r="AE1" s="100" t="s">
-        <v>19</v>
+        <v>341</v>
       </c>
       <c r="AF1" s="301" t="s">
         <v>28</v>
@@ -9197,7 +9200,7 @@
         <v>81</v>
       </c>
       <c r="AH3" s="330">
-        <f t="shared" ref="AH2:AH11" si="3">IF(AG3&gt;0,AG3*703/X3^2,0)</f>
+        <f t="shared" ref="AH3:AH11" si="3">IF(AG3&gt;0,AG3*703/X3^2,0)</f>
         <v>26.910680529300567</v>
       </c>
       <c r="AI3" s="330">
@@ -19408,65 +19411,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="64" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="447" t="s">
+      <c r="A1" s="366" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="448"/>
-      <c r="C1" s="449"/>
-      <c r="D1" s="450" t="s">
+      <c r="B1" s="367"/>
+      <c r="C1" s="368"/>
+      <c r="D1" s="369" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="451"/>
-      <c r="F1" s="452" t="s">
+      <c r="E1" s="370"/>
+      <c r="F1" s="371" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="453"/>
-      <c r="H1" s="454"/>
-      <c r="I1" s="455" t="s">
+      <c r="G1" s="372"/>
+      <c r="H1" s="373"/>
+      <c r="I1" s="374" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="456"/>
-      <c r="K1" s="457"/>
-      <c r="L1" s="458" t="s">
+      <c r="J1" s="375"/>
+      <c r="K1" s="376"/>
+      <c r="L1" s="377" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="459"/>
+      <c r="M1" s="378"/>
       <c r="N1" s="101"/>
-      <c r="O1" s="432" t="s">
+      <c r="O1" s="384" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="433"/>
-      <c r="Q1" s="433"/>
-      <c r="R1" s="434"/>
-      <c r="S1" s="439" t="s">
+      <c r="P1" s="385"/>
+      <c r="Q1" s="385"/>
+      <c r="R1" s="386"/>
+      <c r="S1" s="393" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="440"/>
-      <c r="U1" s="440"/>
-      <c r="V1" s="440"/>
-      <c r="W1" s="440"/>
-      <c r="X1" s="440"/>
-      <c r="Y1" s="440"/>
-      <c r="Z1" s="440"/>
-      <c r="AA1" s="440"/>
-      <c r="AB1" s="440"/>
-      <c r="AC1" s="440"/>
-      <c r="AD1" s="441"/>
-      <c r="AE1" s="442" t="s">
+      <c r="T1" s="394"/>
+      <c r="U1" s="394"/>
+      <c r="V1" s="394"/>
+      <c r="W1" s="394"/>
+      <c r="X1" s="394"/>
+      <c r="Y1" s="394"/>
+      <c r="Z1" s="394"/>
+      <c r="AA1" s="394"/>
+      <c r="AB1" s="394"/>
+      <c r="AC1" s="394"/>
+      <c r="AD1" s="395"/>
+      <c r="AE1" s="396" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="443"/>
-      <c r="AG1" s="444"/>
-      <c r="AH1" s="445" t="s">
+      <c r="AF1" s="397"/>
+      <c r="AG1" s="398"/>
+      <c r="AH1" s="399" t="s">
         <v>123</v>
       </c>
-      <c r="AI1" s="446"/>
-      <c r="AJ1" s="446"/>
-      <c r="AK1" s="429" t="s">
+      <c r="AI1" s="400"/>
+      <c r="AJ1" s="400"/>
+      <c r="AK1" s="379" t="s">
         <v>124</v>
       </c>
-      <c r="AL1" s="430"/>
-      <c r="AM1" s="431"/>
+      <c r="AL1" s="380"/>
+      <c r="AM1" s="381"/>
     </row>
     <row r="2" spans="1:39" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
@@ -19520,10 +19523,10 @@
         <f>M2/$B$6</f>
         <v>1</v>
       </c>
-      <c r="O2" s="380" t="s">
+      <c r="O2" s="382" t="s">
         <v>129</v>
       </c>
-      <c r="P2" s="381"/>
+      <c r="P2" s="383"/>
       <c r="Q2" s="109">
         <f>COUNTIF('CLIENT LIST'!S2:S11,"&gt;=130")</f>
         <v>3</v>
@@ -19545,19 +19548,19 @@
         <v>132</v>
       </c>
       <c r="Y2" s="84"/>
-      <c r="Z2" s="432" t="s">
+      <c r="Z2" s="384" t="s">
         <v>130</v>
       </c>
-      <c r="AA2" s="433"/>
-      <c r="AB2" s="434"/>
+      <c r="AA2" s="385"/>
+      <c r="AB2" s="386"/>
       <c r="AC2" s="115"/>
       <c r="AD2" s="360" t="s">
         <v>133</v>
       </c>
-      <c r="AE2" s="435" t="s">
+      <c r="AE2" s="387" t="s">
         <v>134</v>
       </c>
-      <c r="AF2" s="436"/>
+      <c r="AF2" s="388"/>
       <c r="AG2" s="116">
         <f>COUNTIF('CLIENT LIST'!$AM$2:$AM$11,"X")</f>
         <v>4</v>
@@ -19637,10 +19640,10 @@
         <f t="shared" ref="N3:N6" si="2">M3/$B$6</f>
         <v>1</v>
       </c>
-      <c r="O3" s="380" t="s">
+      <c r="O3" s="382" t="s">
         <v>139</v>
       </c>
-      <c r="P3" s="381"/>
+      <c r="P3" s="383"/>
       <c r="Q3" s="109">
         <f>COUNTIF('CLIENT LIST'!T2:T11,"&gt;=90")</f>
         <v>2</v>
@@ -19664,10 +19667,10 @@
       <c r="W3" s="124"/>
       <c r="X3" s="123"/>
       <c r="Y3" s="125"/>
-      <c r="Z3" s="437" t="s">
+      <c r="Z3" s="389" t="s">
         <v>140</v>
       </c>
-      <c r="AA3" s="438"/>
+      <c r="AA3" s="390"/>
       <c r="AB3" s="126">
         <f>COUNTIFS('CLIENT LIST'!AH2:AH11,"&lt;18",'CLIENT LIST'!AH2:AH11,"&gt;0")</f>
         <v>0</v>
@@ -19680,10 +19683,10 @@
         <f>AB3-T3</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="393" t="s">
+      <c r="AE3" s="391" t="s">
         <v>35</v>
       </c>
-      <c r="AF3" s="394"/>
+      <c r="AF3" s="392"/>
       <c r="AG3" s="116">
         <f>COUNTIF('CLIENT LIST'!$AN$2:$AN$11,"X")</f>
         <v>4</v>
@@ -19760,10 +19763,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O4" s="380" t="s">
+      <c r="O4" s="382" t="s">
         <v>144</v>
       </c>
-      <c r="P4" s="381"/>
+      <c r="P4" s="383"/>
       <c r="Q4" s="109">
         <f>COUNTIF('CLIENT LIST'!U2:U11,"&gt;=200")</f>
         <v>1</v>
@@ -19787,10 +19790,10 @@
       <c r="W4" s="136"/>
       <c r="X4" s="135"/>
       <c r="Y4" s="137"/>
-      <c r="Z4" s="425" t="s">
+      <c r="Z4" s="401" t="s">
         <v>145</v>
       </c>
-      <c r="AA4" s="426"/>
+      <c r="AA4" s="402"/>
       <c r="AB4" s="126">
         <f>COUNTIFS('CLIENT LIST'!AH2:AH11,"&gt;=18",'CLIENT LIST'!AH2:AH11,"&lt;25")</f>
         <v>1</v>
@@ -19803,10 +19806,10 @@
         <f>AB4-T4</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="393" t="s">
+      <c r="AE4" s="391" t="s">
         <v>146</v>
       </c>
-      <c r="AF4" s="394"/>
+      <c r="AF4" s="392"/>
       <c r="AG4" s="116">
         <f>COUNTIF('CLIENT LIST'!$AO$2:$AO$11,"X")</f>
         <v>4</v>
@@ -19835,10 +19838,10 @@
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="427" t="s">
+      <c r="A5" s="403" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="428"/>
+      <c r="B5" s="404"/>
       <c r="C5" s="139"/>
       <c r="D5" s="104" t="s">
         <v>77</v>
@@ -19880,10 +19883,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O5" s="380" t="s">
+      <c r="O5" s="382" t="s">
         <v>150</v>
       </c>
-      <c r="P5" s="381"/>
+      <c r="P5" s="383"/>
       <c r="Q5" s="109">
         <f>COUNTIF('CLIENT LIST'!W2:W11,"&gt;=200")</f>
         <v>1</v>
@@ -19913,10 +19916,10 @@
         <v>0</v>
       </c>
       <c r="Y5" s="143"/>
-      <c r="Z5" s="417" t="s">
+      <c r="Z5" s="405" t="s">
         <v>151</v>
       </c>
-      <c r="AA5" s="418"/>
+      <c r="AA5" s="406"/>
       <c r="AB5" s="144">
         <f>COUNTIFS('CLIENT LIST'!AH2:AH11,"&gt;=25",'CLIENT LIST'!AH2:AH11,"&lt;30")</f>
         <v>1</v>
@@ -19929,10 +19932,10 @@
         <f>AB5-T5</f>
         <v>0</v>
       </c>
-      <c r="AE5" s="393" t="s">
+      <c r="AE5" s="391" t="s">
         <v>37</v>
       </c>
-      <c r="AF5" s="394"/>
+      <c r="AF5" s="392"/>
       <c r="AG5" s="116">
         <f>COUNTIF('CLIENT LIST'!$AP$2:$AP$11,"X")</f>
         <v>1</v>
@@ -20010,10 +20013,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O6" s="380" t="s">
+      <c r="O6" s="382" t="s">
         <v>155</v>
       </c>
-      <c r="P6" s="381"/>
+      <c r="P6" s="383"/>
       <c r="Q6" s="149">
         <f>COUNTIF('CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>3</v>
@@ -20043,10 +20046,10 @@
         <v>1</v>
       </c>
       <c r="Y6" s="143"/>
-      <c r="Z6" s="417" t="s">
+      <c r="Z6" s="405" t="s">
         <v>156</v>
       </c>
-      <c r="AA6" s="418"/>
+      <c r="AA6" s="406"/>
       <c r="AB6" s="144">
         <f>COUNTIFS('CLIENT LIST'!$AH$2:$AH$11,"&gt;=30",'CLIENT LIST'!$AH$2:$AH$11,"&lt;40")</f>
         <v>2</v>
@@ -20059,10 +20062,10 @@
         <f>AB6-T6</f>
         <v>1</v>
       </c>
-      <c r="AE6" s="393" t="s">
+      <c r="AE6" s="391" t="s">
         <v>38</v>
       </c>
-      <c r="AF6" s="394"/>
+      <c r="AF6" s="392"/>
       <c r="AG6" s="116">
         <f>COUNTIF('CLIENT LIST'!$AQ$2:$AQ$11,"X")</f>
         <v>1</v>
@@ -20120,15 +20123,15 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="L7" s="408" t="s">
+      <c r="L7" s="411" t="s">
         <v>159</v>
       </c>
-      <c r="M7" s="409"/>
-      <c r="N7" s="410"/>
-      <c r="O7" s="419" t="s">
+      <c r="M7" s="412"/>
+      <c r="N7" s="413"/>
+      <c r="O7" s="414" t="s">
         <v>160</v>
       </c>
-      <c r="P7" s="420"/>
+      <c r="P7" s="415"/>
       <c r="Q7" s="104">
         <f>COUNTIF('CLIENT LIST'!AA2:AA11,"&gt;=5.7")</f>
         <v>2</v>
@@ -20158,10 +20161,10 @@
         <v>0</v>
       </c>
       <c r="Y7" s="137"/>
-      <c r="Z7" s="421" t="s">
+      <c r="Z7" s="416" t="s">
         <v>161</v>
       </c>
-      <c r="AA7" s="422"/>
+      <c r="AA7" s="417"/>
       <c r="AB7" s="159">
         <f>COUNTIFS('CLIENT LIST'!$AH$2:$AH$11,"&gt;40")</f>
         <v>0</v>
@@ -20174,10 +20177,10 @@
         <f>AB7-T7</f>
         <v>-1</v>
       </c>
-      <c r="AE7" s="393" t="s">
+      <c r="AE7" s="391" t="s">
         <v>162</v>
       </c>
-      <c r="AF7" s="394"/>
+      <c r="AF7" s="392"/>
       <c r="AG7" s="116">
         <f>COUNTIF('CLIENT LIST'!$AR$2:$AR$11,"X")</f>
         <v>1</v>
@@ -20246,11 +20249,11 @@
         <f>M8/$B$6</f>
         <v>1</v>
       </c>
-      <c r="O8" s="423" t="s">
+      <c r="O8" s="407" t="s">
         <v>165</v>
       </c>
-      <c r="P8" s="424"/>
-      <c r="Q8" s="424"/>
+      <c r="P8" s="408"/>
+      <c r="Q8" s="408"/>
       <c r="R8" s="61"/>
       <c r="S8" s="162"/>
       <c r="T8" s="163">
@@ -20270,10 +20273,10 @@
       </c>
       <c r="AC8" s="147"/>
       <c r="AD8" s="147"/>
-      <c r="AE8" s="393" t="s">
+      <c r="AE8" s="391" t="s">
         <v>166</v>
       </c>
-      <c r="AF8" s="394"/>
+      <c r="AF8" s="392"/>
       <c r="AG8" s="116">
         <f>COUNTIF('CLIENT LIST'!$AS$2:$AS$11,"X")</f>
         <v>1</v>
@@ -20330,15 +20333,15 @@
       <c r="L9" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="M9" s="371">
+      <c r="M9" s="428">
         <f>SUMIF('CLIENT LIST'!$BD$2:$BD$11,"&lt;0")</f>
         <v>-11</v>
       </c>
-      <c r="N9" s="372"/>
-      <c r="O9" s="380" t="s">
+      <c r="N9" s="429"/>
+      <c r="O9" s="382" t="s">
         <v>169</v>
       </c>
-      <c r="P9" s="381"/>
+      <c r="P9" s="383"/>
       <c r="Q9" s="109">
         <f>COUNTIFS('CLIENT LIST'!U2:U11,"&gt;=200",'CLIENT LIST'!S2:S11,"&gt;=140")</f>
         <v>1</v>
@@ -20364,19 +20367,19 @@
         <v>132</v>
       </c>
       <c r="Y9" s="84"/>
-      <c r="Z9" s="369" t="s">
+      <c r="Z9" s="409" t="s">
         <v>173</v>
       </c>
-      <c r="AA9" s="370"/>
-      <c r="AB9" s="377" t="s">
+      <c r="AA9" s="410"/>
+      <c r="AB9" s="430" t="s">
         <v>174</v>
       </c>
       <c r="AC9" s="147"/>
       <c r="AD9" s="147"/>
-      <c r="AE9" s="393" t="s">
+      <c r="AE9" s="391" t="s">
         <v>41</v>
       </c>
-      <c r="AF9" s="394"/>
+      <c r="AF9" s="392"/>
       <c r="AG9" s="116">
         <f>COUNTIF('CLIENT LIST'!$AT$2:$AT$11,"X")</f>
         <v>1</v>
@@ -20397,15 +20400,15 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="388" t="s">
+      <c r="A10" s="418" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="390"/>
+      <c r="B10" s="419"/>
       <c r="C10" s="355"/>
-      <c r="D10" s="403" t="s">
+      <c r="D10" s="420" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="403" t="s">
+      <c r="E10" s="420" t="s">
         <v>177</v>
       </c>
       <c r="F10" s="147"/>
@@ -20420,15 +20423,15 @@
       <c r="L10" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="M10" s="371">
+      <c r="M10" s="428">
         <f>AVERAGEIF('CLIENT LIST'!$BD$2:$BD$11,"&lt;0")</f>
         <v>-5.5</v>
       </c>
-      <c r="N10" s="372"/>
-      <c r="O10" s="380" t="s">
+      <c r="N10" s="429"/>
+      <c r="O10" s="382" t="s">
         <v>179</v>
       </c>
-      <c r="P10" s="381"/>
+      <c r="P10" s="383"/>
       <c r="Q10" s="126">
         <f>COUNTIFS('CLIENT LIST'!W2:W11,"&gt;=140",'CLIENT LIST'!S2:S11,"&gt;=140")</f>
         <v>1</v>
@@ -20448,23 +20451,23 @@
         <f>COUNTIF('CLIENT LIST'!T2:T11,"&lt;=79")</f>
         <v>1</v>
       </c>
-      <c r="V10" s="414" t="s">
+      <c r="V10" s="432" t="s">
         <v>181</v>
       </c>
-      <c r="W10" s="415"/>
-      <c r="X10" s="415"/>
-      <c r="Y10" s="416"/>
+      <c r="W10" s="433"/>
+      <c r="X10" s="433"/>
+      <c r="Y10" s="434"/>
       <c r="Z10" s="168" t="s">
         <v>182</v>
       </c>
       <c r="AA10" s="359"/>
-      <c r="AB10" s="379"/>
+      <c r="AB10" s="431"/>
       <c r="AC10" s="160"/>
       <c r="AD10" s="147"/>
-      <c r="AE10" s="393" t="s">
+      <c r="AE10" s="391" t="s">
         <v>42</v>
       </c>
-      <c r="AF10" s="394"/>
+      <c r="AF10" s="392"/>
       <c r="AG10" s="116">
         <f>COUNTIF('CLIENT LIST'!$AU$2:$AU$11,"X")</f>
         <v>1</v>
@@ -20493,25 +20496,25 @@
         <f>B11/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D11" s="404"/>
-      <c r="E11" s="406"/>
+      <c r="D11" s="421"/>
+      <c r="E11" s="423"/>
       <c r="F11" s="147"/>
       <c r="G11" s="147"/>
       <c r="H11" s="147"/>
-      <c r="I11" s="411" t="s">
+      <c r="I11" s="425" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="412"/>
-      <c r="K11" s="413"/>
-      <c r="L11" s="408" t="s">
+      <c r="J11" s="426"/>
+      <c r="K11" s="427"/>
+      <c r="L11" s="411" t="s">
         <v>183</v>
       </c>
-      <c r="M11" s="409"/>
-      <c r="N11" s="410"/>
-      <c r="O11" s="380" t="s">
+      <c r="M11" s="412"/>
+      <c r="N11" s="413"/>
+      <c r="O11" s="382" t="s">
         <v>184</v>
       </c>
-      <c r="P11" s="381"/>
+      <c r="P11" s="383"/>
       <c r="Q11" s="126">
         <f>COUNTIFS('CLIENT LIST'!S2:S11,"&gt;=140",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>2</v>
@@ -20554,10 +20557,10 @@
       </c>
       <c r="AC11" s="173"/>
       <c r="AD11" s="147"/>
-      <c r="AE11" s="393" t="s">
+      <c r="AE11" s="391" t="s">
         <v>43</v>
       </c>
-      <c r="AF11" s="394"/>
+      <c r="AF11" s="392"/>
       <c r="AG11" s="116">
         <f>COUNTIF('CLIENT LIST'!$AV$2:$AV$11,"X")</f>
         <v>0</v>
@@ -20581,8 +20584,8 @@
         <f t="shared" ref="C12:C31" si="7">B12/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D12" s="405"/>
-      <c r="E12" s="407"/>
+      <c r="D12" s="422"/>
+      <c r="E12" s="424"/>
       <c r="F12" s="147"/>
       <c r="G12" s="147"/>
       <c r="H12" s="147"/>
@@ -20608,10 +20611,10 @@
         <f>M12/$B$6</f>
         <v>1</v>
       </c>
-      <c r="O12" s="380" t="s">
+      <c r="O12" s="382" t="s">
         <v>188</v>
       </c>
-      <c r="P12" s="381"/>
+      <c r="P12" s="383"/>
       <c r="Q12" s="126">
         <f>COUNTIFS('CLIENT LIST'!S2:S11,"&gt;=140",'CLIENT LIST'!W2:W11,"&gt;=140",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>1</v>
@@ -20654,10 +20657,10 @@
       </c>
       <c r="AC12" s="173"/>
       <c r="AD12" s="147"/>
-      <c r="AE12" s="393" t="s">
+      <c r="AE12" s="391" t="s">
         <v>44</v>
       </c>
-      <c r="AF12" s="394"/>
+      <c r="AF12" s="392"/>
       <c r="AG12" s="116">
         <f>COUNTIF('CLIENT LIST'!$AW$2:$AW$11,"X")</f>
         <v>1</v>
@@ -20706,15 +20709,15 @@
       <c r="L13" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="M13" s="391">
+      <c r="M13" s="436">
         <f>SUMIF('CLIENT LIST'!$BF$2:$BF$11,"&lt;0")</f>
         <v>-5.7295042438271615</v>
       </c>
-      <c r="N13" s="392"/>
-      <c r="O13" s="395" t="s">
+      <c r="N13" s="437"/>
+      <c r="O13" s="438" t="s">
         <v>192</v>
       </c>
-      <c r="P13" s="396"/>
+      <c r="P13" s="439"/>
       <c r="Q13" s="126">
         <f>COUNTIFS('CLIENT LIST'!U2:U11,"&gt;=200",'CLIENT LIST'!S2:S11,"&gt;=140",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>1</v>
@@ -20757,10 +20760,10 @@
       </c>
       <c r="AC13" s="173"/>
       <c r="AD13" s="147"/>
-      <c r="AE13" s="393" t="s">
+      <c r="AE13" s="391" t="s">
         <v>194</v>
       </c>
-      <c r="AF13" s="394"/>
+      <c r="AF13" s="392"/>
       <c r="AG13" s="116">
         <f>COUNTIF('CLIENT LIST'!$AX$2:$AX$11,"X")</f>
         <v>1</v>
@@ -20794,7 +20797,7 @@
       </c>
       <c r="F14" s="147"/>
       <c r="G14" s="147"/>
-      <c r="H14" s="402" t="s">
+      <c r="H14" s="447" t="s">
         <v>339</v>
       </c>
       <c r="I14" s="180" t="s">
@@ -20811,15 +20814,15 @@
       <c r="L14" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="M14" s="391">
+      <c r="M14" s="436">
         <f>AVERAGEIF('CLIENT LIST'!$BF$2:$BF$11,"&lt;0")</f>
         <v>-2.8647521219135808</v>
       </c>
-      <c r="N14" s="392"/>
-      <c r="O14" s="380" t="s">
+      <c r="N14" s="437"/>
+      <c r="O14" s="382" t="s">
         <v>195</v>
       </c>
-      <c r="P14" s="381"/>
+      <c r="P14" s="383"/>
       <c r="Q14" s="126">
         <f>COUNTIFS('CLIENT LIST'!W2:W11,"&gt;=140",'CLIENT LIST'!U2:U11,"&gt;=200")</f>
         <v>1</v>
@@ -20851,10 +20854,10 @@
       </c>
       <c r="AC14" s="160"/>
       <c r="AD14" s="147"/>
-      <c r="AE14" s="400" t="s">
+      <c r="AE14" s="443" t="s">
         <v>46</v>
       </c>
-      <c r="AF14" s="401"/>
+      <c r="AF14" s="444"/>
       <c r="AG14" s="116">
         <f>COUNTIF('CLIENT LIST'!$AY$2:$AY$11,"X")</f>
         <v>1</v>
@@ -20878,15 +20881,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D15" s="388" t="s">
+      <c r="D15" s="418" t="s">
         <v>197</v>
       </c>
-      <c r="E15" s="389"/>
-      <c r="F15" s="390"/>
+      <c r="E15" s="435"/>
+      <c r="F15" s="419"/>
       <c r="G15" s="160" t="s">
         <v>198</v>
       </c>
-      <c r="H15" s="402"/>
+      <c r="H15" s="447"/>
       <c r="I15" s="190" t="s">
         <v>85</v>
       </c>
@@ -20898,15 +20901,15 @@
         <f>J15/$B$4</f>
         <v>0.25</v>
       </c>
-      <c r="L15" s="397" t="s">
+      <c r="L15" s="440" t="s">
         <v>199</v>
       </c>
-      <c r="M15" s="398"/>
-      <c r="N15" s="399"/>
-      <c r="O15" s="380" t="s">
+      <c r="M15" s="441"/>
+      <c r="N15" s="442"/>
+      <c r="O15" s="382" t="s">
         <v>200</v>
       </c>
-      <c r="P15" s="381"/>
+      <c r="P15" s="383"/>
       <c r="Q15" s="126">
         <f>COUNTIFS('CLIENT LIST'!U2:U11,"&gt;=200",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>1</v>
@@ -20915,10 +20918,10 @@
         <f>Q15/$B$4</f>
         <v>0.25</v>
       </c>
-      <c r="S15" s="384" t="s">
+      <c r="S15" s="445" t="s">
         <v>201</v>
       </c>
-      <c r="T15" s="385"/>
+      <c r="T15" s="446"/>
       <c r="U15" s="192"/>
       <c r="V15" s="147"/>
       <c r="W15" s="147"/>
@@ -20998,10 +21001,10 @@
         <f t="shared" ref="N16" si="10">M16/$B$6</f>
         <v>0.5</v>
       </c>
-      <c r="O16" s="380" t="s">
+      <c r="O16" s="382" t="s">
         <v>203</v>
       </c>
-      <c r="P16" s="381"/>
+      <c r="P16" s="383"/>
       <c r="Q16" s="126">
         <f>COUNTIFS('CLIENT LIST'!W2:W11,"&gt;=140",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>2</v>
@@ -21023,10 +21026,10 @@
         <v>132</v>
       </c>
       <c r="Y16" s="84"/>
-      <c r="Z16" s="369" t="s">
+      <c r="Z16" s="409" t="s">
         <v>173</v>
       </c>
-      <c r="AA16" s="370"/>
+      <c r="AA16" s="410"/>
       <c r="AB16" s="147"/>
       <c r="AC16" s="147"/>
       <c r="AD16" s="147"/>
@@ -21081,15 +21084,15 @@
       <c r="L17" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="M17" s="371">
+      <c r="M17" s="428">
         <f>SUMIF('CLIENT LIST'!$BD$2:$BD$11,"&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="N17" s="372"/>
-      <c r="O17" s="373" t="s">
+      <c r="N17" s="429"/>
+      <c r="O17" s="456" t="s">
         <v>206</v>
       </c>
-      <c r="P17" s="374"/>
+      <c r="P17" s="457"/>
       <c r="Q17" s="159">
         <f>COUNTIFS('CLIENT LIST'!U2:U11,"&gt;=200",'CLIENT LIST'!S2:S11,"&gt;=140",'CLIENT LIST'!W2:W11,"&gt;=140",'CLIENT LIST'!Z2:Z11,"&gt;=25")</f>
         <v>1</v>
@@ -21113,10 +21116,10 @@
       <c r="W17" s="206"/>
       <c r="X17" s="206"/>
       <c r="Y17" s="206"/>
-      <c r="Z17" s="375" t="s">
+      <c r="Z17" s="458" t="s">
         <v>207</v>
       </c>
-      <c r="AA17" s="376"/>
+      <c r="AA17" s="459"/>
       <c r="AB17" s="105">
         <f>SUM(AB18,AB19,AB20,AB21)</f>
         <v>1</v>
@@ -21169,11 +21172,11 @@
       <c r="L18" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="M18" s="371">
+      <c r="M18" s="428">
         <f>AVERAGEIF('CLIENT LIST'!$BD$2:$BD$11,"&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="N18" s="372"/>
+      <c r="N18" s="429"/>
       <c r="O18" s="147"/>
       <c r="P18" s="147"/>
       <c r="Q18" s="147"/>
@@ -21475,10 +21478,10 @@
       <c r="P22" s="147"/>
       <c r="Q22" s="147"/>
       <c r="R22" s="147"/>
-      <c r="S22" s="369" t="s">
+      <c r="S22" s="409" t="s">
         <v>201</v>
       </c>
-      <c r="T22" s="370"/>
+      <c r="T22" s="410"/>
       <c r="U22" s="147"/>
       <c r="V22" s="147"/>
       <c r="W22" s="147"/>
@@ -21527,10 +21530,10 @@
       <c r="P23" s="147"/>
       <c r="Q23" s="147"/>
       <c r="R23" s="147"/>
-      <c r="S23" s="382" t="s">
+      <c r="S23" s="449" t="s">
         <v>207</v>
       </c>
-      <c r="T23" s="383"/>
+      <c r="T23" s="450"/>
       <c r="U23" s="105"/>
       <c r="V23" s="113" t="s">
         <v>131</v>
@@ -21845,10 +21848,10 @@
       <c r="P29" s="147"/>
       <c r="Q29" s="147"/>
       <c r="R29" s="147"/>
-      <c r="S29" s="384" t="s">
+      <c r="S29" s="445" t="s">
         <v>215</v>
       </c>
-      <c r="T29" s="385"/>
+      <c r="T29" s="446"/>
       <c r="U29" s="147"/>
       <c r="V29" s="147"/>
       <c r="W29" s="147"/>
@@ -21889,10 +21892,10 @@
       <c r="P30" s="147"/>
       <c r="Q30" s="147"/>
       <c r="R30" s="147"/>
-      <c r="S30" s="386" t="s">
+      <c r="S30" s="451" t="s">
         <v>24</v>
       </c>
-      <c r="T30" s="387"/>
+      <c r="T30" s="452"/>
       <c r="U30" s="227"/>
       <c r="V30" s="201" t="s">
         <v>131</v>
@@ -21945,12 +21948,12 @@
         <v>0</v>
       </c>
       <c r="U31" s="113"/>
-      <c r="V31" s="366" t="s">
+      <c r="V31" s="453" t="s">
         <v>218</v>
       </c>
-      <c r="W31" s="367"/>
-      <c r="X31" s="367"/>
-      <c r="Y31" s="368"/>
+      <c r="W31" s="454"/>
+      <c r="X31" s="454"/>
+      <c r="Y31" s="455"/>
       <c r="Z31" s="147"/>
       <c r="AA31" s="147"/>
       <c r="AB31" s="147"/>
@@ -22082,7 +22085,7 @@
       <c r="AF35" s="147"/>
     </row>
     <row r="36" spans="19:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="S36" s="377" t="s">
+      <c r="S36" s="430" t="s">
         <v>222</v>
       </c>
       <c r="T36" s="235"/>
@@ -22099,7 +22102,7 @@
       <c r="AE36" s="147"/>
     </row>
     <row r="37" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S37" s="378"/>
+      <c r="S37" s="448"/>
       <c r="T37" s="147"/>
       <c r="U37" s="147"/>
       <c r="V37" s="147"/>
@@ -22114,7 +22117,7 @@
       <c r="AE37" s="147"/>
     </row>
     <row r="38" spans="19:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="S38" s="379"/>
+      <c r="S38" s="431"/>
       <c r="T38" s="147"/>
       <c r="U38" s="147"/>
       <c r="V38" s="147"/>
@@ -27667,53 +27670,18 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="S1:AD1"/>
-    <mergeCell ref="AE1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="V31:Y31"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S36:S38"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="O12:P12"/>
@@ -27728,18 +27696,53 @@
     <mergeCell ref="O15:P15"/>
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="S36:S38"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="V31:Y31"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="AB11:AB14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
@@ -27779,11 +27782,11 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="461" t="s">
+      <c r="A3" s="468" t="s">
         <v>272</v>
       </c>
-      <c r="B3" s="461"/>
-      <c r="C3" s="461"/>
+      <c r="B3" s="468"/>
+      <c r="C3" s="468"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
@@ -27799,11 +27802,11 @@
     </row>
     <row r="7" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="462" t="s">
+      <c r="B7" s="469" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="463"/>
-      <c r="D7" s="464"/>
+      <c r="C7" s="470"/>
+      <c r="D7" s="471"/>
       <c r="E7" s="8">
         <f>COUNTIF('CLIENT LIST'!H2:H11,"M")</f>
         <v>3</v>
@@ -27813,11 +27816,11 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="462" t="s">
+      <c r="K7" s="469" t="s">
         <v>275</v>
       </c>
-      <c r="L7" s="463"/>
-      <c r="M7" s="464"/>
+      <c r="L7" s="470"/>
+      <c r="M7" s="471"/>
       <c r="N7" s="8">
         <f>COUNTIF('CLIENT LIST'!H2:H11,"F")</f>
         <v>1</v>
@@ -27828,26 +27831,26 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="465" t="s">
+      <c r="B8" s="464" t="s">
         <v>276</v>
       </c>
-      <c r="C8" s="466"/>
-      <c r="D8" s="466"/>
-      <c r="E8" s="466"/>
-      <c r="F8" s="466"/>
-      <c r="G8" s="466"/>
-      <c r="H8" s="466"/>
+      <c r="C8" s="465"/>
+      <c r="D8" s="465"/>
+      <c r="E8" s="465"/>
+      <c r="F8" s="465"/>
+      <c r="G8" s="465"/>
+      <c r="H8" s="465"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="467" t="s">
+      <c r="K8" s="466" t="s">
         <v>277</v>
       </c>
-      <c r="L8" s="466"/>
-      <c r="M8" s="466"/>
-      <c r="N8" s="466"/>
-      <c r="O8" s="466"/>
-      <c r="P8" s="466"/>
-      <c r="Q8" s="466"/>
+      <c r="L8" s="465"/>
+      <c r="M8" s="465"/>
+      <c r="N8" s="465"/>
+      <c r="O8" s="465"/>
+      <c r="P8" s="465"/>
+      <c r="Q8" s="465"/>
       <c r="R8" s="362"/>
       <c r="S8" s="13"/>
       <c r="T8" s="14"/>
@@ -27856,22 +27859,22 @@
       <c r="A9" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B9" s="460"/>
-      <c r="C9" s="460"/>
-      <c r="D9" s="460"/>
-      <c r="E9" s="460"/>
-      <c r="F9" s="460"/>
-      <c r="G9" s="460"/>
-      <c r="H9" s="460"/>
+      <c r="B9" s="467"/>
+      <c r="C9" s="467"/>
+      <c r="D9" s="467"/>
+      <c r="E9" s="467"/>
+      <c r="F9" s="467"/>
+      <c r="G9" s="467"/>
+      <c r="H9" s="467"/>
       <c r="I9" s="361"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="460"/>
-      <c r="L9" s="460"/>
-      <c r="M9" s="460"/>
-      <c r="N9" s="460"/>
-      <c r="O9" s="460"/>
-      <c r="P9" s="460"/>
-      <c r="Q9" s="460"/>
+      <c r="K9" s="467"/>
+      <c r="L9" s="467"/>
+      <c r="M9" s="467"/>
+      <c r="N9" s="467"/>
+      <c r="O9" s="467"/>
+      <c r="P9" s="467"/>
+      <c r="Q9" s="467"/>
       <c r="R9" s="361"/>
       <c r="S9" s="361"/>
       <c r="T9" s="9"/>
@@ -28409,10 +28412,10 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="468" t="s">
+      <c r="G20" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="469"/>
+      <c r="H20" s="463"/>
       <c r="I20" s="29">
         <f>$E$7-I19</f>
         <v>0</v>
@@ -28423,10 +28426,10 @@
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
-      <c r="P20" s="468" t="s">
+      <c r="P20" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="Q20" s="469"/>
+      <c r="Q20" s="463"/>
       <c r="R20" s="29">
         <f>$N$7-R19</f>
         <v>0</v>
@@ -28436,26 +28439,26 @@
     </row>
     <row r="21" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="465" t="s">
+      <c r="B21" s="464" t="s">
         <v>276</v>
       </c>
-      <c r="C21" s="466"/>
-      <c r="D21" s="466"/>
-      <c r="E21" s="466"/>
-      <c r="F21" s="466"/>
-      <c r="G21" s="466"/>
-      <c r="H21" s="466"/>
+      <c r="C21" s="465"/>
+      <c r="D21" s="465"/>
+      <c r="E21" s="465"/>
+      <c r="F21" s="465"/>
+      <c r="G21" s="465"/>
+      <c r="H21" s="465"/>
       <c r="I21" s="362"/>
       <c r="J21" s="12"/>
-      <c r="K21" s="467" t="s">
+      <c r="K21" s="466" t="s">
         <v>277</v>
       </c>
-      <c r="L21" s="466"/>
-      <c r="M21" s="466"/>
-      <c r="N21" s="466"/>
-      <c r="O21" s="466"/>
-      <c r="P21" s="466"/>
-      <c r="Q21" s="466"/>
+      <c r="L21" s="465"/>
+      <c r="M21" s="465"/>
+      <c r="N21" s="465"/>
+      <c r="O21" s="465"/>
+      <c r="P21" s="465"/>
+      <c r="Q21" s="465"/>
       <c r="R21" s="362"/>
       <c r="S21" s="13"/>
       <c r="T21" s="14"/>
@@ -28464,22 +28467,22 @@
       <c r="A22" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B22" s="460"/>
-      <c r="C22" s="460"/>
-      <c r="D22" s="460"/>
-      <c r="E22" s="460"/>
-      <c r="F22" s="460"/>
-      <c r="G22" s="460"/>
-      <c r="H22" s="460"/>
+      <c r="B22" s="467"/>
+      <c r="C22" s="467"/>
+      <c r="D22" s="467"/>
+      <c r="E22" s="467"/>
+      <c r="F22" s="467"/>
+      <c r="G22" s="467"/>
+      <c r="H22" s="467"/>
       <c r="I22" s="361"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="460"/>
-      <c r="L22" s="460"/>
-      <c r="M22" s="460"/>
-      <c r="N22" s="460"/>
-      <c r="O22" s="460"/>
-      <c r="P22" s="460"/>
-      <c r="Q22" s="460"/>
+      <c r="K22" s="467"/>
+      <c r="L22" s="467"/>
+      <c r="M22" s="467"/>
+      <c r="N22" s="467"/>
+      <c r="O22" s="467"/>
+      <c r="P22" s="467"/>
+      <c r="Q22" s="467"/>
       <c r="R22" s="361"/>
       <c r="S22" s="361"/>
       <c r="T22" s="9"/>
@@ -28801,10 +28804,10 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="468" t="s">
+      <c r="G29" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="469"/>
+      <c r="H29" s="463"/>
       <c r="I29" s="29">
         <f>$E$7-I28</f>
         <v>0</v>
@@ -28815,10 +28818,10 @@
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="468" t="s">
+      <c r="P29" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="Q29" s="469"/>
+      <c r="Q29" s="463"/>
       <c r="R29" s="29">
         <f>$N$7-R28</f>
         <v>0</v>
@@ -28827,26 +28830,26 @@
       <c r="T29" s="33"/>
     </row>
     <row r="30" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="465" t="s">
+      <c r="B30" s="464" t="s">
         <v>276</v>
       </c>
-      <c r="C30" s="466"/>
-      <c r="D30" s="466"/>
-      <c r="E30" s="466"/>
-      <c r="F30" s="466"/>
-      <c r="G30" s="466"/>
-      <c r="H30" s="466"/>
+      <c r="C30" s="465"/>
+      <c r="D30" s="465"/>
+      <c r="E30" s="465"/>
+      <c r="F30" s="465"/>
+      <c r="G30" s="465"/>
+      <c r="H30" s="465"/>
       <c r="I30" s="362"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="467" t="s">
+      <c r="K30" s="466" t="s">
         <v>277</v>
       </c>
-      <c r="L30" s="466"/>
-      <c r="M30" s="466"/>
-      <c r="N30" s="466"/>
-      <c r="O30" s="466"/>
-      <c r="P30" s="466"/>
-      <c r="Q30" s="466"/>
+      <c r="L30" s="465"/>
+      <c r="M30" s="465"/>
+      <c r="N30" s="465"/>
+      <c r="O30" s="465"/>
+      <c r="P30" s="465"/>
+      <c r="Q30" s="465"/>
       <c r="R30" s="362"/>
       <c r="S30" s="13"/>
       <c r="T30" s="14"/>
@@ -28855,22 +28858,22 @@
       <c r="A31" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B31" s="460"/>
-      <c r="C31" s="460"/>
-      <c r="D31" s="460"/>
-      <c r="E31" s="460"/>
-      <c r="F31" s="460"/>
-      <c r="G31" s="460"/>
-      <c r="H31" s="460"/>
+      <c r="B31" s="467"/>
+      <c r="C31" s="467"/>
+      <c r="D31" s="467"/>
+      <c r="E31" s="467"/>
+      <c r="F31" s="467"/>
+      <c r="G31" s="467"/>
+      <c r="H31" s="467"/>
       <c r="I31" s="361"/>
       <c r="J31" s="9"/>
-      <c r="K31" s="460"/>
-      <c r="L31" s="460"/>
-      <c r="M31" s="460"/>
-      <c r="N31" s="460"/>
-      <c r="O31" s="460"/>
-      <c r="P31" s="460"/>
-      <c r="Q31" s="460"/>
+      <c r="K31" s="467"/>
+      <c r="L31" s="467"/>
+      <c r="M31" s="467"/>
+      <c r="N31" s="467"/>
+      <c r="O31" s="467"/>
+      <c r="P31" s="467"/>
+      <c r="Q31" s="467"/>
       <c r="R31" s="361"/>
       <c r="S31" s="361"/>
       <c r="T31" s="9"/>
@@ -29396,10 +29399,10 @@
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="468" t="s">
+      <c r="G42" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="469"/>
+      <c r="H42" s="463"/>
       <c r="I42" s="29">
         <f>$E$7-I41</f>
         <v>0</v>
@@ -29410,10 +29413,10 @@
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
-      <c r="P42" s="468" t="s">
+      <c r="P42" s="462" t="s">
         <v>174</v>
       </c>
-      <c r="Q42" s="469"/>
+      <c r="Q42" s="463"/>
       <c r="R42" s="29">
         <f>$N$7-R41</f>
         <v>0</v>
@@ -29423,26 +29426,26 @@
     </row>
     <row r="43" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
-      <c r="B43" s="465" t="s">
+      <c r="B43" s="464" t="s">
         <v>276</v>
       </c>
-      <c r="C43" s="466"/>
-      <c r="D43" s="466"/>
-      <c r="E43" s="466"/>
-      <c r="F43" s="466"/>
-      <c r="G43" s="466"/>
-      <c r="H43" s="466"/>
+      <c r="C43" s="465"/>
+      <c r="D43" s="465"/>
+      <c r="E43" s="465"/>
+      <c r="F43" s="465"/>
+      <c r="G43" s="465"/>
+      <c r="H43" s="465"/>
       <c r="I43" s="362"/>
       <c r="J43" s="12"/>
-      <c r="K43" s="467" t="s">
+      <c r="K43" s="466" t="s">
         <v>277</v>
       </c>
-      <c r="L43" s="466"/>
-      <c r="M43" s="466"/>
-      <c r="N43" s="466"/>
-      <c r="O43" s="466"/>
-      <c r="P43" s="466"/>
-      <c r="Q43" s="466"/>
+      <c r="L43" s="465"/>
+      <c r="M43" s="465"/>
+      <c r="N43" s="465"/>
+      <c r="O43" s="465"/>
+      <c r="P43" s="465"/>
+      <c r="Q43" s="465"/>
       <c r="R43" s="362"/>
       <c r="S43" s="13"/>
       <c r="T43" s="14"/>
@@ -29451,22 +29454,22 @@
       <c r="A44" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B44" s="460"/>
-      <c r="C44" s="460"/>
-      <c r="D44" s="460"/>
-      <c r="E44" s="460"/>
-      <c r="F44" s="460"/>
-      <c r="G44" s="460"/>
-      <c r="H44" s="460"/>
+      <c r="B44" s="467"/>
+      <c r="C44" s="467"/>
+      <c r="D44" s="467"/>
+      <c r="E44" s="467"/>
+      <c r="F44" s="467"/>
+      <c r="G44" s="467"/>
+      <c r="H44" s="467"/>
       <c r="I44" s="361"/>
       <c r="J44" s="9"/>
-      <c r="K44" s="460"/>
-      <c r="L44" s="460"/>
-      <c r="M44" s="460"/>
-      <c r="N44" s="460"/>
-      <c r="O44" s="460"/>
-      <c r="P44" s="460"/>
-      <c r="Q44" s="460"/>
+      <c r="K44" s="467"/>
+      <c r="L44" s="467"/>
+      <c r="M44" s="467"/>
+      <c r="N44" s="467"/>
+      <c r="O44" s="467"/>
+      <c r="P44" s="467"/>
+      <c r="Q44" s="467"/>
       <c r="R44" s="361"/>
       <c r="S44" s="361"/>
       <c r="T44" s="9"/>
@@ -30599,19 +30602,19 @@
       </c>
     </row>
     <row r="67" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="470" t="s">
+      <c r="G67" s="460" t="s">
         <v>174</v>
       </c>
-      <c r="H67" s="471"/>
+      <c r="H67" s="461"/>
       <c r="I67" s="24">
         <f>$E$7-I66</f>
         <v>0</v>
       </c>
       <c r="J67" s="9"/>
-      <c r="P67" s="470" t="s">
+      <c r="P67" s="460" t="s">
         <v>174</v>
       </c>
-      <c r="Q67" s="471"/>
+      <c r="Q67" s="461"/>
       <c r="R67" s="24">
         <f>$N$7-R66</f>
         <v>0</v>
@@ -30623,6 +30626,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="K8:Q8"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="K21:Q21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="K22:Q22"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="K31:Q31"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="P29:Q29"/>
     <mergeCell ref="G67:H67"/>
     <mergeCell ref="P67:Q67"/>
     <mergeCell ref="G42:H42"/>
@@ -30631,25 +30653,6 @@
     <mergeCell ref="K43:Q43"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="K44:Q44"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="K30:Q30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="K31:Q31"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="K21:Q21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="K22:Q22"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="K9:Q9"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="K8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>